<commit_message>
Deleted line 194: typo that caused import error
This issue was identified by Arnold (Yanuo Zhou) when analysing the data.
</commit_message>
<xml_diff>
--- a/individual/226/continuous/mHLEA_paper/226_mHLEA_paper_20231106.xlsx
+++ b/individual/226/continuous/mHLEA_paper/226_mHLEA_paper_20231106.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="20403"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="20413"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\cyepi\data\raw\individual\226\continuous\mHLEA_paper\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\cguidolin\Downloads\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{EE9B1D94-A78B-4D41-AE0A-1DB4EF4031CA}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{00473AAA-BB12-49F2-B8E8-276EBE3C0327}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="11925" xr2:uid="{368BA072-C6B4-4213-9851-BF656C27EC72}"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="10725" xr2:uid="{368BA072-C6B4-4213-9851-BF656C27EC72}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -427,8 +427,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{18AEBA24-4993-4804-A6A5-43CAEA3CEF26}">
   <dimension ref="A1:D194"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D169" sqref="D169"/>
+    <sheetView tabSelected="1" topLeftCell="A169" workbookViewId="0">
+      <selection activeCell="A194" sqref="A194"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2200,9 +2200,7 @@
       </c>
     </row>
     <row r="194" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A194" s="1">
-        <v>45235.999994444443</v>
-      </c>
+      <c r="A194" s="1"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>